<commit_message>
A lot has gone down...Ex11_2 and Ex13_9 got rekt
</commit_message>
<xml_diff>
--- a/Project4/UML Diagrams Project 4.xlsx
+++ b/Project4/UML Diagrams Project 4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elijahkorneffel/Git/CS2261-JAVA/Project4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662AF96C-2467-B241-AD13-FF0D8D1BA53A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E1445D-0028-C049-80BD-90FD3E261222}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="2240" windowWidth="27300" windowHeight="14900" xr2:uid="{69F5D078-DB60-8645-A592-F6F24EDF1838}"/>
+    <workbookView xWindow="-27320" yWindow="2640" windowWidth="13620" windowHeight="15360" xr2:uid="{69F5D078-DB60-8645-A592-F6F24EDF1838}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,91 +30,166 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>+QuadraticEquation(a: double, b: double, c: double)</t>
-  </si>
-  <si>
-    <t>+getA(): double</t>
-  </si>
-  <si>
-    <t>+getB(): double</t>
-  </si>
-  <si>
-    <t>+getC(): double</t>
-  </si>
-  <si>
-    <t>+getDiscriminant(): double</t>
-  </si>
-  <si>
-    <t>+getRoot1(): double</t>
-  </si>
-  <si>
-    <t>+getRoot2(): double</t>
-  </si>
-  <si>
-    <t>Circle2D</t>
-  </si>
-  <si>
-    <t>-x: double</t>
-  </si>
-  <si>
-    <t>-y: double</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>-name: string</t>
+  </si>
+  <si>
+    <t>-email:string</t>
+  </si>
+  <si>
+    <t>-address: string</t>
+  </si>
+  <si>
+    <t>-phone: string</t>
+  </si>
+  <si>
+    <t>+Person(name: string, address: string, phone: string, email:string)</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>-office: string</t>
+  </si>
+  <si>
+    <t>-salary: string</t>
+  </si>
+  <si>
+    <t>-hired: string</t>
+  </si>
+  <si>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>-rank: string</t>
+  </si>
+  <si>
+    <t>-title: string</t>
+  </si>
+  <si>
+    <t>+Person()</t>
+  </si>
+  <si>
+    <t>+toString(): string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you and she are sperated and she begins to go out, to dance, to enjoy, don't go to that she is fucking since (not sure about this part, dejar doesn’t mean stop here I guess lol) , Think on when you both were together she stopped being herself to be well with you, bruh (I know cabron is something like that lol). Not sure about the stop being free and no le tires ground part. Because when she will be in her house something you don't matter to you. </t>
+  </si>
+  <si>
+    <t>Geometric Object</t>
+  </si>
+  <si>
+    <t>Circle</t>
+  </si>
+  <si>
+    <t>-classStatus: string</t>
+  </si>
+  <si>
+    <t>+Employee(name: string, address: string, phone: string, email:string, :string,:string:string,)</t>
+  </si>
+  <si>
+    <t>-dateHired: string</t>
+  </si>
+  <si>
+    <t>-hours: string</t>
+  </si>
+  <si>
+    <t>+Faculty(name: string, address: string, phone: string, email:string, hours: string, rank: string)</t>
+  </si>
+  <si>
+    <t>+Staff(name: string, address: string, phone: string, email:string, title: string)</t>
+  </si>
+  <si>
+    <t>+Student(name: string, address: string, phone: string, email:string, classStatus: string)</t>
+  </si>
+  <si>
+    <t>+Employee()</t>
+  </si>
+  <si>
+    <t>-color: String</t>
+  </si>
+  <si>
+    <t>-filled: boolean</t>
+  </si>
+  <si>
+    <t>-dateCreated: java.util.Date</t>
+  </si>
+  <si>
+    <t>#GeomtricObject()</t>
+  </si>
+  <si>
+    <t>#GeometricObject(color: string. Filled: boolean)</t>
+  </si>
+  <si>
+    <t>+getColor(): string</t>
+  </si>
+  <si>
+    <t>+setColor(color: String): void</t>
+  </si>
+  <si>
+    <t>+isFilled(): boolean</t>
+  </si>
+  <si>
+    <t>+setFilled(filled: boolean): void</t>
+  </si>
+  <si>
+    <t>+getDateCreated(): java.util.Date</t>
+  </si>
+  <si>
+    <t>+toString(): String</t>
   </si>
   <si>
     <t>-radius: double</t>
   </si>
   <si>
-    <t>+getX(): double</t>
-  </si>
-  <si>
-    <t>+getY(): double</t>
+    <t>+Circle()</t>
+  </si>
+  <si>
+    <t>+Circle(radius: double)</t>
+  </si>
+  <si>
+    <t>+Circle(radius: double, color: String, filled: boolean)</t>
   </si>
   <si>
     <t>+getRadius(): double</t>
   </si>
   <si>
+    <t>+setRadius(radius: double): void</t>
+  </si>
+  <si>
     <t>+getArea(): double</t>
   </si>
   <si>
     <t>+getPerimeter(): double</t>
   </si>
   <si>
-    <t>+contains(circle: Circle2D): boolean</t>
-  </si>
-  <si>
-    <t>+contains(x: double, y: double): boolean</t>
-  </si>
-  <si>
-    <t>+overlaps(circle: Circle2D): boolean</t>
-  </si>
-  <si>
-    <t>+Circle2D()</t>
-  </si>
-  <si>
-    <t>+Circle2D(x: double, y: double, radius: double)</t>
-  </si>
-  <si>
-    <t>Person</t>
-  </si>
-  <si>
-    <t>-name: string</t>
-  </si>
-  <si>
-    <t>-email:string</t>
-  </si>
-  <si>
-    <t>-address: string</t>
-  </si>
-  <si>
-    <t>-phone: string</t>
+    <t>+getDiameter(): double</t>
+  </si>
+  <si>
+    <t>+printCircle(): void</t>
+  </si>
+  <si>
+    <t>+equalt(o:Object): boolean</t>
+  </si>
+  <si>
+    <t>+compareTo(o: Circle): int</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -136,8 +211,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,8 +244,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -257,11 +345,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF70AD47"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -281,6 +378,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -296,6 +404,471 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>422960</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>101200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>112980</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>176840</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="5" name="Ink 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3842D6CF-C305-5F46-B40C-5C83B7C31BB2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2073960" y="2565000"/>
+            <a:ext cx="515520" cy="482040"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="5" name="Ink 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3842D6CF-C305-5F46-B40C-5C83B7C31BB2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2065320" y="2556360"/>
+              <a:ext cx="533160" cy="499680"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>216620</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>112360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>805900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>112040</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="6" name="Ink 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55795AC1-FC6F-AB45-93C1-72A555C08585}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="4344120" y="2576160"/>
+            <a:ext cx="2240280" cy="406080"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="6" name="Ink 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55795AC1-FC6F-AB45-93C1-72A555C08585}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4335480" y="2567520"/>
+              <a:ext cx="2257920" cy="423720"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>82740</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>118720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>656580</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>18420</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="7" name="Ink 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44418FCC-F615-6747-8170-4324811A74E8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2559240" y="5020920"/>
+            <a:ext cx="573840" cy="522000"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="7" name="Ink 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44418FCC-F615-6747-8170-4324811A74E8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2550600" y="5013824"/>
+              <a:ext cx="591480" cy="535909"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>147500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>180280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>65380</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>203000</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="8" name="Ink 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3A88BD6-0934-DE49-A08C-18DBDD2D67EE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="4275000" y="5082480"/>
+            <a:ext cx="1568880" cy="429120"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="8" name="Ink 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3A88BD6-0934-DE49-A08C-18DBDD2D67EE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4266000" y="5074760"/>
+              <a:ext cx="1586520" cy="444882"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>179600</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>50240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>653360</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>156120</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="9" name="Ink 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3A77F7E-173D-014F-873A-F027158B5EE4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="1830600" y="9626040"/>
+            <a:ext cx="473760" cy="512280"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="9" name="Ink 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3A77F7E-173D-014F-873A-F027158B5EE4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1821600" y="9617400"/>
+              <a:ext cx="491400" cy="529920"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-17T05:44:21.926"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">722 1339 24575,'0'-19'0,"0"-18"0,0-14 0,0-14 0,-5 8 0,-3-15 0,-4 13 0,-2-15 0,1 10 0,-4 6 0,8 9 0,-12 3 0,13 11 0,-8-5 0,5 13 0,5 0 0,-3 1 0,7 5 0,-7-11 0,7 11 0,-7-11 0,8 5 0,-4-7 0,-1-5 0,5 4 0,-10-12 0,10 12 0,-10-11 0,10 11 0,-9 1 0,9 8 0,-8 6 0,8 4 0,-3 2 0,4 5 0,-4 4 0,-1 1 0,0 7 0,1 2 0,4 4 0,0 0 0,-4 0 0,3 5 0,-7-4 0,3 9 0,-9-4 0,2 11 0,-7-4 0,2 9 0,-10-2 0,4-1 0,-12 6 0,6-5 0,0 6 0,-6 0 0,6 0 0,-1-1 0,-5 2 0,13-8 0,-6-1 0,13-7 0,-4-4 0,8-2 0,1-4 0,6-1 0,0-4 0,3-5 0,-3-10 0,4-5 0,5-5 0,-4 0 0,8-1 0,-3-5 0,4 5 0,6-11 0,-4 5 0,9-6 0,-4-1 0,0 7 0,3 1 0,-9 6 0,8-1 0,-3 1 0,4 4 0,1-3 0,5 3 0,-5-5 0,11-1 0,-10 2 0,9-2 0,-9 6 0,-1 1 0,-2 0 0,-8 9 0,3-7 0,-5 12 0,0-7 0,0 7 0,0-4 0,0 5 0,0 0 0,5 0 0,-3 0 0,8 0 0,-4 0 0,6 0 0,-1 0 0,0 9 0,0-2 0,6 13 0,-4-4 0,4 4 0,0 1 0,1 1 0,1-1 0,3 1 0,-2 5 0,11-2 0,-2 9 0,8-9 0,-1 11 0,3-10 0,4 11 0,-3-11 0,-6 4 0,4-7 0,-13 0 0,1-6 0,-4-1 0,-14-6 0,3 0 0,-11-1 0,0 0 0,1-4 0,-5-1 0,-1-4 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-17T05:44:25.934"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">6223 1128 24575,'-30'0'0,"-20"0"0,-10 0 0,-22 0 0,-3 0-1117,-10 0 1117,43 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,1 0 0,-1 0 0,-1 0 0,-4 0 0,0 0 0,4 0 0,-1 0 0,-3 0 0,-1 0 0,0 0 0,1 0 0,2 0 0,3 0-69,-32 0 69,30 0 0,1 0 0,-13 0 0,16 0 0,-3 0 0,-40 0 0,40-3 0,0-1 0,0 4 0,0-2 0,-4-4 0,0-1 0,5-1 0,0 1 0,0-1 0,0-1-436,-6-2 0,1 0 436,-2-1 0,0 1 0,-5 3 0,0-2 0,0-5 0,1 0 0,-1 6 0,0 0 0,0-6 0,0 0 0,0 6 0,0 0 0,0-5 0,1-2 0,-1 4 0,1 0 0,0 0 0,-1-1 0,1-2 0,0 0 0,-1 6 0,0 0 0,0-2 0,0-1 0,1 0 0,-1 1 0,-6 2 0,1 0 0,3-3 0,1 1 0,9 3 0,1 0 0,-1 1 0,2-1 0,-33-6 0,35 7 0,1-1 0,-45-6 0,5 0 0,7-1-131,9 2 131,1-1 785,17 2-785,1-6 339,8 4-339,7-3 919,1 6-919,7 0 146,5 0-146,3 0 0,5 1 0,0 0 0,4 4 0,-3-3 0,9 4 0,-4-5 0,0 1 0,4-1 0,-9 0 0,4 0 0,-5 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-9-5 0,7 4 0,-7-4 0,9 5 0,0-1 0,-6 1 0,4-1 0,-4-4 0,6 4 0,0-4 0,0 5 0,0 0 0,5 0 0,1 5 0,5 1 0,4 0 0,-3 3 0,7 4 0,-3 3 0,8 11 0,2 4 0,5 13 0,1 14 0,1 1 0,-1 14 0,1-6 0,0 8 0,6 0 0,-5-7 0,4-9 0,-6-10 0,-1-6 0,-5-5 0,3-7 0,-4-7 0,0-5 0,4 5 0,-8-4 0,8 4 0,-4-5 0,4 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,-4 0 0,4 0 0,-8 0 0,7-4 0,-7-5 0,3-10 0,-4 0 0,0-9 0,0 4 0,0-5 0,0-1 0,-5-5 0,-1-1 0,-5-6 0,-6-7 0,5 5 0,-11-11 0,11 5 0,-11-8 0,10 8 0,-4-6 0,1 12 0,3-4 0,-3-1 0,5 11 0,0-10 0,1 18 0,-1-5 0,1 5 0,0 1 0,0 5 0,5 1 0,-3 4 0,3 2 0,0-1 0,1 0 0,4 1 0,-4 3 0,3-3 0,-7 7 0,7-7 0,-7 3 0,3-4 0,-4-6 0,-1 0 0,0 0 0,5 1 0,-4 0 0,4 3 0,0-3 0,1 5 0,7 4 0,2 5 0,9 6 0,-4-1 0,10 4 0,1-3 0,0-1 0,11 5 0,2-3 0,8 4 0,6 1 0,0 0 0,8 1 0,9-6 0,2 4 0,13-10 0,-13 11 0,15-11 0,-14 5 0,14-6 0,-15 0 0,6 0 0,-7 0 0,-9 0 0,7 0 0,-15 0 0,7 0 0,-15 0 0,5 0 0,-4 0 0,0 0 0,4 0 0,-4 0 0,-1 0 0,6 0 0,-12 0 0,-1 0 0,-3 0 0,-14 0 0,8 0 0,-15 0 0,4 0 0,-5 0 0,-11 0 0,1-4 0,-8 3 0,5-3 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-17T05:44:29.818"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">600 1839 24575,'0'-33'0,"0"3"0,0-39 0,0 22 0,0-41 0,0 30 0,0-14 0,0 13 0,0 15 0,0-6 0,0 7 0,0 9 0,0-7 0,0 14 0,0-13 0,0 5 0,0-7 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 7 0,-5-5 0,4 5 0,-4-15 0,5 6 0,0-7 0,0 9 0,0-8 0,-5 13 0,4-12 0,-3 22 0,-1-6 0,4 13 0,-3 2 0,0 7 0,-1 4 0,-3 2 0,0 5 0,3 5 0,-3 1 0,7 12 0,-7 1 0,7 14 0,-8-6 0,3 13 0,-5 4 0,-5 0 0,-3 14 0,-5 5 0,-6 1 0,-3 17 0,-6-14 0,0 14 0,0-13 0,-7 15 0,5-14 0,-6 7 0,16-21 0,1-2 0,9-19 0,5-7 0,6-9 0,2-7 0,7 1 0,-3-15 0,4-6 0,0-15 0,0-9 0,5-1 0,1-9 0,10 1 0,1 0 0,5 0 0,7-2 0,-5 2 0,4-2 0,-1 8 0,-4-4 0,10 2 0,-10 3 0,12-9 0,-12 9 0,11-10 0,-4 0 0,6-1 0,1 0 0,0-9 0,0 7 0,-6-5 0,-3 9 0,-6 3 0,0 6 0,-6 2 0,-1 13 0,-5-4 0,-1 11 0,0-5 0,0 12 0,0 1 0,-1 5 0,1 0 0,0 5 0,0 2 0,11 11 0,2 3 0,11 7 0,8 9 0,-4 1 0,12 3 0,-12 3 0,12-3 0,-11 5 0,4-7 0,-12 3 0,2-12 0,-10 3 0,10-5 0,-11-3 0,5-4 0,-5 3 0,5-9 0,-5 9 0,0-10 0,-2 5 0,-3-7 0,-1 0 0,4 1 0,-8-2 0,3 1 0,-5 0 0,0-6 0,0 4 0,1-8 0,-1 8 0,5-9 0,-4 4 0,5-5 0,-1 0 0,-4 0 0,4 0 0,-5 0 0,-3 0 0,-2 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-17T05:44:33.446"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">4357 1334 24575,'-28'0'0,"-8"0"0,-12 0 0,-10-13 0,-6 4 0,-9-20 0,-3 5 0,1 0 0,-7 1 0,15 2 0,-25 11 0,15-17-573,-17 16 573,1-12 0,40 14 0,0 1 0,-28-1 0,31-2 0,1 0 0,-28 0 0,-19-12 0,44 10 0,-1 1 0,-42-6 0,2-6 0,17 3 0,3 4 0,8-4 0,0 6 0,7 1 0,3 6 0,-1-5 0,7 6 573,-14-1-573,13-4 0,-6 4 0,1-6 0,5 6 0,-6-4 0,8 4 0,0-5 0,0 5 0,0-4 0,0 11 0,-21-11 0,16 4 0,-16 1 0,20-5 0,1 10 0,0-10 0,7 5 0,-6-6 0,13 0 0,-6 0 0,7 1 0,0 0 0,0-1 0,0-5 0,0 4 0,6-3 0,-5 4 0,5-4 0,-6 3 0,0-4 0,6 1 0,-5 3 0,5-8 0,-6 8 0,6-3 0,-5-1 0,11 5 0,-11-5 0,10 2 0,-9 2 0,9-2 0,-9-2 0,9 5 0,-10-10 0,11 10 0,-5-10 0,6 11 0,-6-10 0,5 9 0,-5-10 0,6 11 0,0-10 0,-6 9 0,4-9 0,-4 9 0,2-13 0,3 12 0,1-7 0,6 10 0,5 6 0,0 0 0,0 5 0,4 4 0,1 2 0,4 3 0,0 1 0,5 6 0,0-4 0,5 9 0,0-4 0,6 12 0,-4 9 0,10 8 0,-3 8 0,6 8 0,0 2 0,-5 8 0,3-9 0,-3 8 0,5-15 0,0 6 0,-7-8 0,4-8 0,-9-1 0,3-8 0,0 0 0,-3 0 0,2-7 0,-5-7 0,0-1 0,0-11 0,-5 5 0,-1-6 0,-4 0 0,0-13 0,0-4 0,0-14 0,0-8 0,0 4 0,0-4 0,-5 0 0,-1-2 0,-5-6 0,0 0 0,-5-7 0,3-2 0,-4-1 0,0-5 0,4 5 0,-4 1 0,6 1 0,0 8 0,-1 0 0,2 6 0,-1-4 0,1 10 0,-1-4 0,1 7 0,1 5 0,3-5 0,-2 11 0,3-5 0,0 0 0,-3 4 0,7-3 0,-7 4 0,7 1 0,-7 0 0,3-1 0,0 1 0,-3 4 0,3-3 0,0 3 0,-3-4 0,3 0 0,0 0 0,-2 5 0,6-4 0,-3 4 0,4-5 0,0 1 0,0-1 0,4 5 0,1 1 0,3 4 0,2 0 0,-1 0 0,0 4 0,0 2 0,1 4 0,4 1 0,1-1 0,5-3 0,1 3 0,5-9 0,1 4 0,6 0 0,7-3 0,-5 3 0,11-5 0,-4 0 0,-1 0 0,6 0 0,-12 0 0,4 0 0,-5 0 0,-1 0 0,0 0 0,-5 0 0,3 0 0,-4 0 0,1 0 0,3 0 0,-9 0 0,13 0 0,-13 0 0,8 0 0,-10 0 0,-5 0 0,-1 0 0,-4 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,-8 0 0,-1 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink5.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-17T05:45:01.860"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">529 1423 24575,'0'-12'0,"0"-9"0,0-5 0,0-14 0,0-9 0,0-1 0,0-6 0,0 8 0,0 0 0,0 0 0,0-7 0,0 5 0,0-5 0,0 7 0,0-16 0,-11 11 0,8-18 0,-19 13 0,19-7 0,-14 7 0,11 2 0,-1 8 0,-3 7 0,9-5 0,-9 11 0,9 1 0,-9 2 0,9 16 0,-4-9 0,5 14 0,-4 1 0,-1 6 0,1 8 0,-4 1 0,7 4 0,-3 0 0,0-1 0,3 2 0,-7-1 0,7 5 0,-8 1 0,4 5 0,-5 0 0,-6 6 0,-1 8 0,-6 7 0,-1 7 0,-7 8 0,5 1 0,-12 3 0,11 3 0,-11-4 0,12-3 0,-4-7 0,12-9 0,3-12 0,5-8 0,4-6 0,-2-4 0,7-1 0,-3-8 0,4-7 0,0-9 0,0 0 0,0-10 0,0 8 0,0-9 0,0 6 0,5 0 0,1-6 0,4-2 0,1-5 0,1 0 0,-1 0 0,0 0 0,0 6 0,5-5 0,-5 4 0,5 1 0,-1 1 0,-3 6 0,3-6 0,-5 4 0,5-4 0,2 0 0,4-1 0,2-13 0,-1 5 0,1-5 0,0 7 0,-7 5 0,4 2 0,-8 6 0,2 5 0,-4 1 0,-1 9 0,-4-4 0,3 8 0,-4 1 0,1 5 0,-1 4 0,-4 0 0,4 5 0,2-4 0,4 15 0,10-13 0,5 20 0,9-13 0,0 9 0,8 2 0,0-5 0,10 12 0,-4-12 0,3 13 0,-2-13 0,1 6 0,-7-2 0,3-4 0,-9 4 0,3-6 0,-7-1 0,0-5 0,-6 3 0,5-3 0,-10-1 0,4 3 0,-6-7 0,-5 2 0,-1-5 0,-4-4 0,-1 3 0,0-7 0,-4 3 0,-1-4 0</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -595,261 +1168,614 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A50911-3036-7F42-BDAC-A2567F0FBB86}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:13" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="M7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+    <row r="9" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="12" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
+      <c r="G13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="15" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="12"/>
+    </row>
+    <row r="14" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="3"/>
+      <c r="G14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" ht="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="3"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="3"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" ht="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="1:11" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="15"/>
+      <c r="G18" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="15"/>
+      <c r="G19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="3"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="23" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="12"/>
+      <c r="G25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>15</v>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" ht="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="G27" s="7"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="9"/>
+    </row>
+    <row r="28" spans="1:11" ht="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
+      <c r="G28" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="15"/>
+    </row>
+    <row r="29" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15"/>
+      <c r="G29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="3"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="1:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="33" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="6"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="12"/>
+    </row>
+    <row r="35" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" ht="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" ht="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="9"/>
+    </row>
+    <row r="39" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A39" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="15"/>
+    </row>
+    <row r="40" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A40" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="15"/>
+    </row>
+    <row r="41" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="4"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="50" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="12"/>
+    </row>
+    <row r="52" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="1:5" ht="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" ht="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="7"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="9"/>
+    </row>
+    <row r="55" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A55" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="15"/>
+    </row>
+    <row r="56" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A64" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A65" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="1:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="4"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="17">
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="G28:K28"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A55:E55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>